<commit_message>
Correciones fechas en Y y deporar archivo manual
</commit_message>
<xml_diff>
--- a/Data/Input/Calendario.xlsx
+++ b/Data/Input/Calendario.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="107" documentId="11_876FAEB6EA86ADBEEBA0B4032E314CBE899607E2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0A11107-01BB-4C89-81E7-357C2C396328}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-19335" yWindow="-2340" windowWidth="19470" windowHeight="15030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19335" yWindow="-2340" windowWidth="19470" windowHeight="15030"/>
   </bookViews>
   <sheets>
     <sheet name="Calendario fidelización" sheetId="1" r:id="rId1"/>
@@ -13,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Calendario fidelización'!$A$1:$F$366</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -275,8 +274,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,6 +287,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -319,13 +326,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,27 +614,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:F385"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>78</v>
       </c>
@@ -645,7 +654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44562</v>
       </c>
@@ -653,7 +662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44563</v>
       </c>
@@ -661,7 +670,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44564</v>
       </c>
@@ -669,7 +678,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44565</v>
       </c>
@@ -677,7 +686,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44566</v>
       </c>
@@ -685,7 +694,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44567</v>
       </c>
@@ -693,7 +702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44568</v>
       </c>
@@ -701,7 +710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44569</v>
       </c>
@@ -709,15 +718,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44570</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44571</v>
       </c>
@@ -725,7 +735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44572</v>
       </c>
@@ -733,7 +743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44573</v>
       </c>
@@ -753,7 +763,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44574</v>
       </c>
@@ -761,7 +771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44575</v>
       </c>
@@ -769,7 +779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44576</v>
       </c>
@@ -777,7 +787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44577</v>
       </c>
@@ -785,7 +795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44578</v>
       </c>
@@ -793,7 +803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44579</v>
       </c>
@@ -801,7 +811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44580</v>
       </c>
@@ -809,7 +819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44581</v>
       </c>
@@ -829,7 +839,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44582</v>
       </c>
@@ -837,7 +847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44583</v>
       </c>
@@ -845,7 +855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44584</v>
       </c>
@@ -853,7 +863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44585</v>
       </c>
@@ -861,7 +871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44586</v>
       </c>
@@ -869,7 +879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44587</v>
       </c>
@@ -877,7 +887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44588</v>
       </c>
@@ -897,7 +907,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44589</v>
       </c>
@@ -905,7 +915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44590</v>
       </c>
@@ -913,7 +923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44591</v>
       </c>
@@ -921,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44592</v>
       </c>
@@ -929,7 +939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44593</v>
       </c>
@@ -937,7 +947,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44594</v>
       </c>
@@ -945,7 +955,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44595</v>
       </c>
@@ -953,7 +963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44596</v>
       </c>
@@ -961,7 +971,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44597</v>
       </c>
@@ -969,7 +979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44598</v>
       </c>
@@ -977,7 +987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44599</v>
       </c>
@@ -985,7 +995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44600</v>
       </c>
@@ -993,7 +1003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44601</v>
       </c>
@@ -1001,7 +1011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44602</v>
       </c>
@@ -1009,7 +1019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44603</v>
       </c>
@@ -1017,7 +1027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44604</v>
       </c>
@@ -1037,7 +1047,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44605</v>
       </c>
@@ -1045,7 +1055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44606</v>
       </c>
@@ -1053,7 +1063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44607</v>
       </c>
@@ -1061,7 +1071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44608</v>
       </c>
@@ -1069,7 +1079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44609</v>
       </c>
@@ -1077,7 +1087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44610</v>
       </c>
@@ -1085,7 +1095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44611</v>
       </c>
@@ -1093,7 +1103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44612</v>
       </c>
@@ -1113,7 +1123,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44613</v>
       </c>
@@ -1121,7 +1131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44614</v>
       </c>
@@ -1129,7 +1139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44615</v>
       </c>
@@ -1137,7 +1147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44616</v>
       </c>
@@ -1145,7 +1155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44617</v>
       </c>
@@ -1153,7 +1163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44618</v>
       </c>
@@ -1161,7 +1171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44619</v>
       </c>
@@ -1181,7 +1191,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44620</v>
       </c>
@@ -1189,7 +1199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>44621</v>
       </c>
@@ -1197,7 +1207,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>44622</v>
       </c>
@@ -1205,7 +1215,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>44623</v>
       </c>
@@ -1213,7 +1223,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>44624</v>
       </c>
@@ -1221,7 +1231,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>44625</v>
       </c>
@@ -1229,7 +1239,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>44626</v>
       </c>
@@ -1237,7 +1247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>44627</v>
       </c>
@@ -1245,7 +1255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44628</v>
       </c>
@@ -1253,7 +1263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>44629</v>
       </c>
@@ -1261,7 +1271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>44630</v>
       </c>
@@ -1269,7 +1279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>44631</v>
       </c>
@@ -1277,7 +1287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>44632</v>
       </c>
@@ -1297,7 +1307,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>44633</v>
       </c>
@@ -1305,7 +1315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>44634</v>
       </c>
@@ -1313,7 +1323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>44635</v>
       </c>
@@ -1321,7 +1331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>44636</v>
       </c>
@@ -1329,7 +1339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>44637</v>
       </c>
@@ -1337,7 +1347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>44638</v>
       </c>
@@ -1345,7 +1355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>44639</v>
       </c>
@@ -1353,7 +1363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>44640</v>
       </c>
@@ -1373,7 +1383,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>44641</v>
       </c>
@@ -1381,7 +1391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>44642</v>
       </c>
@@ -1389,7 +1399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>44643</v>
       </c>
@@ -1397,7 +1407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44644</v>
       </c>
@@ -1405,7 +1415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44645</v>
       </c>
@@ -1413,7 +1423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44646</v>
       </c>
@@ -1421,7 +1431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44647</v>
       </c>
@@ -1441,7 +1451,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44648</v>
       </c>
@@ -1449,7 +1459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>44649</v>
       </c>
@@ -1457,7 +1467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>44650</v>
       </c>
@@ -1465,7 +1475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>44651</v>
       </c>
@@ -1473,7 +1483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>44652</v>
       </c>
@@ -1481,7 +1491,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>44653</v>
       </c>
@@ -1489,7 +1499,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>44654</v>
       </c>
@@ -1497,7 +1507,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>44655</v>
       </c>
@@ -1505,7 +1515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>44656</v>
       </c>
@@ -1513,7 +1523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>44657</v>
       </c>
@@ -1521,15 +1531,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>44658</v>
       </c>
       <c r="B98" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F98" s="5"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>44659</v>
       </c>
@@ -1537,7 +1548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>44660</v>
       </c>
@@ -1545,7 +1556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>44661</v>
       </c>
@@ -1553,7 +1564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>44662</v>
       </c>
@@ -1561,7 +1572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>44663</v>
       </c>
@@ -1581,7 +1592,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>44664</v>
       </c>
@@ -1589,7 +1600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>44665</v>
       </c>
@@ -1597,7 +1608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>44666</v>
       </c>
@@ -1605,7 +1616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>44667</v>
       </c>
@@ -1613,7 +1624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>44668</v>
       </c>
@@ -1621,7 +1632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>44669</v>
       </c>
@@ -1629,7 +1640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>44670</v>
       </c>
@@ -1637,7 +1648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>44671</v>
       </c>
@@ -1657,7 +1668,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>44672</v>
       </c>
@@ -1665,7 +1676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>44673</v>
       </c>
@@ -1673,7 +1684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>44674</v>
       </c>
@@ -1681,7 +1692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>44675</v>
       </c>
@@ -1689,7 +1700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>44676</v>
       </c>
@@ -1697,7 +1708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>44677</v>
       </c>
@@ -1705,7 +1716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>44678</v>
       </c>
@@ -1725,7 +1736,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>44679</v>
       </c>
@@ -1733,7 +1744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>44680</v>
       </c>
@@ -1741,7 +1752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>44681</v>
       </c>
@@ -1749,7 +1760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>44682</v>
       </c>
@@ -1757,7 +1768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>44683</v>
       </c>
@@ -1765,7 +1776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>44684</v>
       </c>
@@ -1773,7 +1784,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>44685</v>
       </c>
@@ -1781,7 +1792,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>44686</v>
       </c>
@@ -1789,7 +1800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>44687</v>
       </c>
@@ -1797,7 +1808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>44688</v>
       </c>
@@ -1805,7 +1816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>44689</v>
       </c>
@@ -1813,7 +1824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>44690</v>
       </c>
@@ -1821,7 +1832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>44691</v>
       </c>
@@ -1829,7 +1840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>44692</v>
       </c>
@@ -1837,7 +1848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>44693</v>
       </c>
@@ -1857,7 +1868,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>44694</v>
       </c>
@@ -1865,7 +1876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>44695</v>
       </c>
@@ -1873,7 +1884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>44696</v>
       </c>
@@ -1881,7 +1892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>44697</v>
       </c>
@@ -1889,7 +1900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>44698</v>
       </c>
@@ -1897,7 +1908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>44699</v>
       </c>
@@ -1905,7 +1916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>44700</v>
       </c>
@@ -1913,7 +1924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>44701</v>
       </c>
@@ -1933,7 +1944,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>44702</v>
       </c>
@@ -1941,7 +1952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>44703</v>
       </c>
@@ -1949,7 +1960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>44704</v>
       </c>
@@ -1957,7 +1968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>44705</v>
       </c>
@@ -1965,7 +1976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>44706</v>
       </c>
@@ -1973,7 +1984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>44707</v>
       </c>
@@ -1981,7 +1992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>44708</v>
       </c>
@@ -2001,7 +2012,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>44709</v>
       </c>
@@ -2009,7 +2020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>44710</v>
       </c>
@@ -2017,7 +2028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>44711</v>
       </c>
@@ -2025,7 +2036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>44712</v>
       </c>
@@ -2033,7 +2044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>44713</v>
       </c>
@@ -2041,7 +2052,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>44714</v>
       </c>
@@ -2049,7 +2060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>44715</v>
       </c>
@@ -2057,7 +2068,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>44716</v>
       </c>
@@ -2065,7 +2076,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>44717</v>
       </c>
@@ -2073,7 +2084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>44718</v>
       </c>
@@ -2081,7 +2092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>44719</v>
       </c>
@@ -2089,7 +2100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>44720</v>
       </c>
@@ -2097,7 +2108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>44721</v>
       </c>
@@ -2105,7 +2116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>44722</v>
       </c>
@@ -2113,7 +2124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>44723</v>
       </c>
@@ -2121,7 +2132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>44724</v>
       </c>
@@ -2141,7 +2152,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>44725</v>
       </c>
@@ -2149,7 +2160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>44726</v>
       </c>
@@ -2157,7 +2168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>44727</v>
       </c>
@@ -2165,7 +2176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>44728</v>
       </c>
@@ -2173,7 +2184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>44729</v>
       </c>
@@ -2181,7 +2192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>44730</v>
       </c>
@@ -2189,7 +2200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>44731</v>
       </c>
@@ -2197,7 +2208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>44732</v>
       </c>
@@ -2217,7 +2228,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>44733</v>
       </c>
@@ -2225,7 +2236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>44734</v>
       </c>
@@ -2233,7 +2244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>44735</v>
       </c>
@@ -2241,7 +2252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>44736</v>
       </c>
@@ -2249,7 +2260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>44737</v>
       </c>
@@ -2257,7 +2268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>44738</v>
       </c>
@@ -2265,7 +2276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>44739</v>
       </c>
@@ -2285,7 +2296,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>44740</v>
       </c>
@@ -2293,7 +2304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>44741</v>
       </c>
@@ -2301,7 +2312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>44742</v>
       </c>
@@ -2309,7 +2320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>44743</v>
       </c>
@@ -2317,7 +2328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>44744</v>
       </c>
@@ -2325,7 +2336,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>44745</v>
       </c>
@@ -2333,7 +2344,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>44746</v>
       </c>
@@ -2341,7 +2352,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>44747</v>
       </c>
@@ -2349,7 +2360,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>44748</v>
       </c>
@@ -2357,7 +2368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>44749</v>
       </c>
@@ -2365,7 +2376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>44750</v>
       </c>
@@ -2373,7 +2384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>44751</v>
       </c>
@@ -2381,7 +2392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>44752</v>
       </c>
@@ -2389,7 +2400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>44753</v>
       </c>
@@ -2397,7 +2408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>44754</v>
       </c>
@@ -2417,7 +2428,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>44755</v>
       </c>
@@ -2425,7 +2436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>44756</v>
       </c>
@@ -2433,7 +2444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>44757</v>
       </c>
@@ -2441,7 +2452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>44758</v>
       </c>
@@ -2449,7 +2460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>44759</v>
       </c>
@@ -2457,7 +2468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>44760</v>
       </c>
@@ -2465,7 +2476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>44761</v>
       </c>
@@ -2473,7 +2484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>44762</v>
       </c>
@@ -2493,7 +2504,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>44763</v>
       </c>
@@ -2501,7 +2512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>44764</v>
       </c>
@@ -2509,7 +2520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>44765</v>
       </c>
@@ -2517,7 +2528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>44766</v>
       </c>
@@ -2525,7 +2536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>44767</v>
       </c>
@@ -2533,7 +2544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>44768</v>
       </c>
@@ -2541,7 +2552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>44769</v>
       </c>
@@ -2561,7 +2572,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>44770</v>
       </c>
@@ -2569,7 +2580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>44771</v>
       </c>
@@ -2577,7 +2588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>44772</v>
       </c>
@@ -2585,7 +2596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>44773</v>
       </c>
@@ -2593,7 +2604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>44774</v>
       </c>
@@ -2601,7 +2612,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>44775</v>
       </c>
@@ -2609,7 +2620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>44776</v>
       </c>
@@ -2617,7 +2628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>44777</v>
       </c>
@@ -2625,7 +2636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>44778</v>
       </c>
@@ -2633,7 +2644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>44779</v>
       </c>
@@ -2641,7 +2652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>44780</v>
       </c>
@@ -2649,7 +2660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>44781</v>
       </c>
@@ -2657,7 +2668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>44782</v>
       </c>
@@ -2665,7 +2676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>44783</v>
       </c>
@@ -2673,7 +2684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>44784</v>
       </c>
@@ -2681,7 +2692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>44785</v>
       </c>
@@ -2701,7 +2712,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>44786</v>
       </c>
@@ -2709,7 +2720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>44787</v>
       </c>
@@ -2717,7 +2728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>44788</v>
       </c>
@@ -2725,7 +2736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>44789</v>
       </c>
@@ -2733,7 +2744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>44790</v>
       </c>
@@ -2741,7 +2752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>44791</v>
       </c>
@@ -2749,7 +2760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>44792</v>
       </c>
@@ -2757,7 +2768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>44793</v>
       </c>
@@ -2777,7 +2788,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>44794</v>
       </c>
@@ -2785,7 +2796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>44795</v>
       </c>
@@ -2793,7 +2804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>44796</v>
       </c>
@@ -2801,7 +2812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>44797</v>
       </c>
@@ -2809,7 +2820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>44798</v>
       </c>
@@ -2817,7 +2828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>44799</v>
       </c>
@@ -2825,7 +2836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>44800</v>
       </c>
@@ -2845,7 +2856,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>44801</v>
       </c>
@@ -2853,7 +2864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>44802</v>
       </c>
@@ -2861,7 +2872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>44803</v>
       </c>
@@ -2869,7 +2880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>44804</v>
       </c>
@@ -2877,7 +2888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>44805</v>
       </c>
@@ -2885,7 +2896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>44806</v>
       </c>
@@ -2893,7 +2904,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>44807</v>
       </c>
@@ -2901,7 +2912,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>44808</v>
       </c>
@@ -2909,7 +2920,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>44809</v>
       </c>
@@ -2917,7 +2928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>44810</v>
       </c>
@@ -2925,7 +2936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>44811</v>
       </c>
@@ -2933,7 +2944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>44812</v>
       </c>
@@ -2941,7 +2952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>44813</v>
       </c>
@@ -2949,7 +2960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>44814</v>
       </c>
@@ -2957,7 +2968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>44815</v>
       </c>
@@ -2965,7 +2976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>44816</v>
       </c>
@@ -2985,7 +2996,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>44817</v>
       </c>
@@ -2993,7 +3004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>44818</v>
       </c>
@@ -3001,7 +3012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>44819</v>
       </c>
@@ -3009,7 +3020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>44820</v>
       </c>
@@ -3017,7 +3028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>44821</v>
       </c>
@@ -3025,7 +3036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>44822</v>
       </c>
@@ -3033,7 +3044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>44823</v>
       </c>
@@ -3041,7 +3052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>44824</v>
       </c>
@@ -3061,7 +3072,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>44825</v>
       </c>
@@ -3069,7 +3080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>44826</v>
       </c>
@@ -3077,7 +3088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>44827</v>
       </c>
@@ -3085,7 +3096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>44828</v>
       </c>
@@ -3093,7 +3104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>44829</v>
       </c>
@@ -3101,7 +3112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>44830</v>
       </c>
@@ -3109,7 +3120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>44831</v>
       </c>
@@ -3129,7 +3140,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>44832</v>
       </c>
@@ -3137,7 +3148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>44833</v>
       </c>
@@ -3145,7 +3156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>44834</v>
       </c>
@@ -3153,7 +3164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>44835</v>
       </c>
@@ -3161,7 +3172,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>44836</v>
       </c>
@@ -3169,7 +3180,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>44837</v>
       </c>
@@ -3177,7 +3188,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>44838</v>
       </c>
@@ -3185,7 +3196,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>44839</v>
       </c>
@@ -3193,7 +3204,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>44840</v>
       </c>
@@ -3201,7 +3212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>44841</v>
       </c>
@@ -3209,7 +3220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>44842</v>
       </c>
@@ -3217,7 +3228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>44843</v>
       </c>
@@ -3225,7 +3236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>44844</v>
       </c>
@@ -3233,7 +3244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>44845</v>
       </c>
@@ -3241,7 +3252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>44846</v>
       </c>
@@ -3261,7 +3272,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>44847</v>
       </c>
@@ -3269,7 +3280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>44848</v>
       </c>
@@ -3277,7 +3288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>44849</v>
       </c>
@@ -3285,7 +3296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>44850</v>
       </c>
@@ -3293,7 +3304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>44851</v>
       </c>
@@ -3301,7 +3312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>44852</v>
       </c>
@@ -3309,7 +3320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>44853</v>
       </c>
@@ -3317,7 +3328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>44854</v>
       </c>
@@ -3337,7 +3348,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>44855</v>
       </c>
@@ -3345,7 +3356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>44856</v>
       </c>
@@ -3353,7 +3364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>44857</v>
       </c>
@@ -3361,7 +3372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>44858</v>
       </c>
@@ -3369,7 +3380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>44859</v>
       </c>
@@ -3377,7 +3388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>44860</v>
       </c>
@@ -3385,7 +3396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>44861</v>
       </c>
@@ -3405,7 +3416,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>44862</v>
       </c>
@@ -3413,7 +3424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>44863</v>
       </c>
@@ -3421,7 +3432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>44864</v>
       </c>
@@ -3429,7 +3440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>44865</v>
       </c>
@@ -3437,7 +3448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>44866</v>
       </c>
@@ -3445,7 +3456,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>44867</v>
       </c>
@@ -3453,7 +3464,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>44868</v>
       </c>
@@ -3461,7 +3472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>44869</v>
       </c>
@@ -3469,7 +3480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>44870</v>
       </c>
@@ -3477,7 +3488,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>44871</v>
       </c>
@@ -3485,7 +3496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>44872</v>
       </c>
@@ -3493,7 +3504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>44873</v>
       </c>
@@ -3501,7 +3512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>44874</v>
       </c>
@@ -3509,7 +3520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>44875</v>
       </c>
@@ -3517,7 +3528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>44876</v>
       </c>
@@ -3525,7 +3536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <v>44877</v>
       </c>
@@ -3545,7 +3556,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <v>44878</v>
       </c>
@@ -3553,7 +3564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
         <v>44879</v>
       </c>
@@ -3561,7 +3572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
         <v>44880</v>
       </c>
@@ -3569,7 +3580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A321" s="1">
         <v>44881</v>
       </c>
@@ -3577,7 +3588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A322" s="1">
         <v>44882</v>
       </c>
@@ -3585,7 +3596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
         <v>44883</v>
       </c>
@@ -3593,7 +3604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A324" s="1">
         <v>44884</v>
       </c>
@@ -3601,7 +3612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
         <v>44885</v>
       </c>
@@ -3621,7 +3632,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
         <v>44886</v>
       </c>
@@ -3629,7 +3640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A327" s="1">
         <v>44887</v>
       </c>
@@ -3637,7 +3648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A328" s="1">
         <v>44888</v>
       </c>
@@ -3645,7 +3656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A329" s="1">
         <v>44889</v>
       </c>
@@ -3653,7 +3664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A330" s="1">
         <v>44890</v>
       </c>
@@ -3661,7 +3672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A331" s="1">
         <v>44891</v>
       </c>
@@ -3669,7 +3680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A332" s="1">
         <v>44892</v>
       </c>
@@ -3689,7 +3700,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A333" s="1">
         <v>44893</v>
       </c>
@@ -3697,7 +3708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A334" s="1">
         <v>44894</v>
       </c>
@@ -3705,7 +3716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A335" s="1">
         <v>44895</v>
       </c>
@@ -3713,7 +3724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A336" s="1">
         <v>44896</v>
       </c>
@@ -3721,7 +3732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A337" s="1">
         <v>44897</v>
       </c>
@@ -3729,7 +3740,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A338" s="1">
         <v>44898</v>
       </c>
@@ -3737,7 +3748,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="339" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A339" s="1">
         <v>44899</v>
       </c>
@@ -3745,7 +3756,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A340" s="1">
         <v>44900</v>
       </c>
@@ -3753,7 +3764,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A341" s="1">
         <v>44901</v>
       </c>
@@ -3761,7 +3772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A342" s="1">
         <v>44902</v>
       </c>
@@ -3769,7 +3780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A343" s="1">
         <v>44903</v>
       </c>
@@ -3777,7 +3788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A344" s="1">
         <v>44904</v>
       </c>
@@ -3785,7 +3796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A345" s="1">
         <v>44905</v>
       </c>
@@ -3793,7 +3804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A346" s="1">
         <v>44906</v>
       </c>
@@ -3801,7 +3812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A347" s="1">
         <v>44907</v>
       </c>
@@ -3821,7 +3832,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A348" s="1">
         <v>44908</v>
       </c>
@@ -3829,7 +3840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A349" s="1">
         <v>44909</v>
       </c>
@@ -3837,7 +3848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A350" s="1">
         <v>44910</v>
       </c>
@@ -3845,7 +3856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A351" s="1">
         <v>44911</v>
       </c>
@@ -3853,7 +3864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A352" s="1">
         <v>44912</v>
       </c>
@@ -3861,7 +3872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A353" s="1">
         <v>44913</v>
       </c>
@@ -3869,7 +3880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A354" s="1">
         <v>44914</v>
       </c>
@@ -3877,7 +3888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A355" s="1">
         <v>44915</v>
       </c>
@@ -3897,7 +3908,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A356" s="1">
         <v>44916</v>
       </c>
@@ -3905,7 +3916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A357" s="1">
         <v>44917</v>
       </c>
@@ -3913,7 +3924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A358" s="1">
         <v>44918</v>
       </c>
@@ -3921,7 +3932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A359" s="1">
         <v>44919</v>
       </c>
@@ -3929,7 +3940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A360" s="1">
         <v>44920</v>
       </c>
@@ -3937,7 +3948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A361" s="1">
         <v>44921</v>
       </c>
@@ -3945,7 +3956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A362" s="1">
         <v>44922</v>
       </c>
@@ -3965,7 +3976,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A363" s="1">
         <v>44923</v>
       </c>
@@ -3973,7 +3984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A364" s="1">
         <v>44924</v>
       </c>
@@ -3981,7 +3992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A365" s="1">
         <v>44925</v>
       </c>
@@ -3989,7 +4000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A366" s="1">
         <v>44926</v>
       </c>
@@ -3997,81 +4008,82 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A367" s="1"/>
     </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A368" s="1"/>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A369" s="1"/>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A370" s="1"/>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A371" s="1"/>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A372" s="1"/>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A373" s="1"/>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A374" s="1"/>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A375" s="1"/>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376" s="1"/>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A377" s="1"/>
     </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A378" s="1"/>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A379" s="1"/>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A380" s="1"/>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A381" s="1"/>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A382" s="1"/>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383" s="1"/>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A384" s="1"/>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4278,18 +4290,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668E6B46-E1D2-4884-8947-5A667A68A9D5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC537D72-CE20-4DBB-BAE3-4B3C88518F3C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC537D72-CE20-4DBB-BAE3-4B3C88518F3C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668E6B46-E1D2-4884-8947-5A667A68A9D5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Actualización de logs, breaks main y cambio de excel scopes
</commit_message>
<xml_diff>
--- a/Data/Input/Calendario.xlsx
+++ b/Data/Input/Calendario.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-19340" yWindow="-2340" windowWidth="19470" windowHeight="15030"/>
+    <workbookView xWindow="-19335" yWindow="-2340" windowWidth="19470" windowHeight="15030"/>
   </bookViews>
   <sheets>
     <sheet name="Calendario fidelización" sheetId="1" r:id="rId1"/>
@@ -622,19 +622,19 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H112" sqref="H112"/>
+      <selection pane="bottomLeft" activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>78</v>
       </c>
@@ -654,7 +654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44562</v>
       </c>
@@ -662,7 +662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44563</v>
       </c>
@@ -670,7 +670,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44564</v>
       </c>
@@ -678,7 +678,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44565</v>
       </c>
@@ -686,7 +686,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44566</v>
       </c>
@@ -694,7 +694,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44567</v>
       </c>
@@ -702,7 +702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44568</v>
       </c>
@@ -710,7 +710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44569</v>
       </c>
@@ -718,7 +718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44570</v>
       </c>
@@ -727,7 +727,7 @@
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44571</v>
       </c>
@@ -735,7 +735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44572</v>
       </c>
@@ -743,7 +743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44573</v>
       </c>
@@ -763,7 +763,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44574</v>
       </c>
@@ -771,7 +771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44575</v>
       </c>
@@ -779,7 +779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44576</v>
       </c>
@@ -787,7 +787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44577</v>
       </c>
@@ -795,7 +795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44578</v>
       </c>
@@ -803,7 +803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44579</v>
       </c>
@@ -811,7 +811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44580</v>
       </c>
@@ -819,7 +819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44581</v>
       </c>
@@ -839,7 +839,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44582</v>
       </c>
@@ -847,7 +847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44583</v>
       </c>
@@ -855,7 +855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44584</v>
       </c>
@@ -863,7 +863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44585</v>
       </c>
@@ -871,7 +871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44586</v>
       </c>
@@ -879,7 +879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44587</v>
       </c>
@@ -887,7 +887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44588</v>
       </c>
@@ -907,7 +907,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44589</v>
       </c>
@@ -915,7 +915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44590</v>
       </c>
@@ -923,7 +923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44591</v>
       </c>
@@ -931,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44592</v>
       </c>
@@ -939,7 +939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44593</v>
       </c>
@@ -947,7 +947,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44594</v>
       </c>
@@ -955,7 +955,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44595</v>
       </c>
@@ -963,7 +963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44596</v>
       </c>
@@ -971,7 +971,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44597</v>
       </c>
@@ -979,7 +979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44598</v>
       </c>
@@ -987,7 +987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44599</v>
       </c>
@@ -995,7 +995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44600</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44601</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44602</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44603</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44604</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44605</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44606</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44607</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44608</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44609</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44610</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44611</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44612</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44613</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44614</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44615</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44616</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44617</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44618</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44619</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44620</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>44621</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>44622</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>44623</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>44624</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>44625</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>44626</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>44627</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44628</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>44629</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>44630</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>44631</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>44632</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>44633</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>44634</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>44635</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>44636</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>44637</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>44638</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>44639</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>44640</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>44641</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>44642</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>44643</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44644</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44645</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44646</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44647</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44648</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>44649</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>44650</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>44651</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>44652</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>44653</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>44654</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>44655</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>44656</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>44657</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>44658</v>
       </c>
@@ -1540,7 +1540,7 @@
       </c>
       <c r="F98" s="5"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>44659</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>44660</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>44661</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>44662</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>44663</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>44664</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>44665</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>44666</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>44667</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>44668</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>44669</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>44670</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>44671</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>44672</v>
       </c>
@@ -1676,15 +1676,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>44673</v>
       </c>
       <c r="B113" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>44674</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>44675</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>44676</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>44677</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>44678</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>44679</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>44680</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>44681</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>44682</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>44683</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>44684</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>44685</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>44686</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>44687</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>44688</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>44689</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>44690</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>44691</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>44692</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>44693</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>44694</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>44695</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>44696</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>44697</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>44698</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>44699</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>44700</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>44701</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>44702</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>44703</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>44704</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>44705</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>44706</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>44707</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>44708</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>44709</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>44710</v>
       </c>
@@ -2028,7 +2028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>44711</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>44712</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>44713</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>44714</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>44715</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>44716</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>44717</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>44718</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>44719</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>44720</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>44721</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>44722</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>44723</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>44724</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>44725</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>44726</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>44727</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>44728</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>44729</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>44730</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>44731</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>44732</v>
       </c>
@@ -2228,7 +2228,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>44733</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>44734</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>44735</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>44736</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>44737</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>44738</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>44739</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>44740</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>44741</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>44742</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>44743</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>44744</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>44745</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>44746</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>44747</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>44748</v>
       </c>
@@ -2368,7 +2368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>44749</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>44750</v>
       </c>
@@ -2384,7 +2384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>44751</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>44752</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>44753</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>44754</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>44755</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>44756</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>44757</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>44758</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>44759</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>44760</v>
       </c>
@@ -2476,7 +2476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>44761</v>
       </c>
@@ -2484,7 +2484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>44762</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>44763</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>44764</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>44765</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>44766</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>44767</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>44768</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>44769</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>44770</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>44771</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>44772</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>44773</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>44774</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>44775</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>44776</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>44777</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>44778</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>44779</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>44780</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>44781</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>44782</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>44783</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>44784</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>44785</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>44786</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>44787</v>
       </c>
@@ -2728,7 +2728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>44788</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>44789</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>44790</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>44791</v>
       </c>
@@ -2760,7 +2760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>44792</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>44793</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>44794</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>44795</v>
       </c>
@@ -2804,7 +2804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>44796</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>44797</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>44798</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>44799</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>44800</v>
       </c>
@@ -2856,7 +2856,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>44801</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>44802</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>44803</v>
       </c>
@@ -2880,7 +2880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>44804</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>44805</v>
       </c>
@@ -2896,7 +2896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>44806</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>44807</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>44808</v>
       </c>
@@ -2920,7 +2920,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>44809</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>44810</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>44811</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>44812</v>
       </c>
@@ -2952,7 +2952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>44813</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>44814</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>44815</v>
       </c>
@@ -2976,7 +2976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>44816</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>44817</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>44818</v>
       </c>
@@ -3012,7 +3012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>44819</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>44820</v>
       </c>
@@ -3028,7 +3028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>44821</v>
       </c>
@@ -3036,7 +3036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>44822</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>44823</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>44824</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>44825</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>44826</v>
       </c>
@@ -3088,7 +3088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>44827</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>44828</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>44829</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>44830</v>
       </c>
@@ -3120,7 +3120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>44831</v>
       </c>
@@ -3140,7 +3140,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>44832</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>44833</v>
       </c>
@@ -3156,7 +3156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>44834</v>
       </c>
@@ -3164,7 +3164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>44835</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>44836</v>
       </c>
@@ -3180,7 +3180,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>44837</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>44838</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>44839</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>44840</v>
       </c>
@@ -3212,7 +3212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>44841</v>
       </c>
@@ -3220,7 +3220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>44842</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>44843</v>
       </c>
@@ -3236,7 +3236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>44844</v>
       </c>
@@ -3244,7 +3244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>44845</v>
       </c>
@@ -3252,7 +3252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>44846</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>44847</v>
       </c>
@@ -3280,7 +3280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>44848</v>
       </c>
@@ -3288,7 +3288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>44849</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>44850</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>44851</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>44852</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>44853</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>44854</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>44855</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>44856</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>44857</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>44858</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>44859</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>44860</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>44861</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>44862</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>44863</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>44864</v>
       </c>
@@ -3440,7 +3440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>44865</v>
       </c>
@@ -3448,7 +3448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>44866</v>
       </c>
@@ -3456,7 +3456,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>44867</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>44868</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>44869</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>44870</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>44871</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>44872</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>44873</v>
       </c>
@@ -3512,7 +3512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>44874</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>44875</v>
       </c>
@@ -3528,7 +3528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>44876</v>
       </c>
@@ -3536,7 +3536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <v>44877</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <v>44878</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
         <v>44879</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
         <v>44880</v>
       </c>
@@ -3580,7 +3580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A321" s="1">
         <v>44881</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A322" s="1">
         <v>44882</v>
       </c>
@@ -3596,7 +3596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
         <v>44883</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A324" s="1">
         <v>44884</v>
       </c>
@@ -3612,7 +3612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
         <v>44885</v>
       </c>
@@ -3632,7 +3632,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
         <v>44886</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A327" s="1">
         <v>44887</v>
       </c>
@@ -3648,7 +3648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A328" s="1">
         <v>44888</v>
       </c>
@@ -3656,7 +3656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A329" s="1">
         <v>44889</v>
       </c>
@@ -3664,7 +3664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A330" s="1">
         <v>44890</v>
       </c>
@@ -3672,7 +3672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A331" s="1">
         <v>44891</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A332" s="1">
         <v>44892</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A333" s="1">
         <v>44893</v>
       </c>
@@ -3708,7 +3708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A334" s="1">
         <v>44894</v>
       </c>
@@ -3716,7 +3716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A335" s="1">
         <v>44895</v>
       </c>
@@ -3724,7 +3724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A336" s="1">
         <v>44896</v>
       </c>
@@ -3732,7 +3732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A337" s="1">
         <v>44897</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A338" s="1">
         <v>44898</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="339" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A339" s="1">
         <v>44899</v>
       </c>
@@ -3756,7 +3756,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A340" s="1">
         <v>44900</v>
       </c>
@@ -3764,7 +3764,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A341" s="1">
         <v>44901</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A342" s="1">
         <v>44902</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A343" s="1">
         <v>44903</v>
       </c>
@@ -3788,7 +3788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A344" s="1">
         <v>44904</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A345" s="1">
         <v>44905</v>
       </c>
@@ -3804,7 +3804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A346" s="1">
         <v>44906</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A347" s="1">
         <v>44907</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A348" s="1">
         <v>44908</v>
       </c>
@@ -3840,7 +3840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A349" s="1">
         <v>44909</v>
       </c>
@@ -3848,7 +3848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A350" s="1">
         <v>44910</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A351" s="1">
         <v>44911</v>
       </c>
@@ -3864,7 +3864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A352" s="1">
         <v>44912</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A353" s="1">
         <v>44913</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A354" s="1">
         <v>44914</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A355" s="1">
         <v>44915</v>
       </c>
@@ -3908,7 +3908,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A356" s="1">
         <v>44916</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A357" s="1">
         <v>44917</v>
       </c>
@@ -3924,7 +3924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A358" s="1">
         <v>44918</v>
       </c>
@@ -3932,7 +3932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A359" s="1">
         <v>44919</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A360" s="1">
         <v>44920</v>
       </c>
@@ -3948,7 +3948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A361" s="1">
         <v>44921</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A362" s="1">
         <v>44922</v>
       </c>
@@ -3976,7 +3976,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A363" s="1">
         <v>44923</v>
       </c>
@@ -3984,7 +3984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A364" s="1">
         <v>44924</v>
       </c>
@@ -3992,7 +3992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A365" s="1">
         <v>44925</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A366" s="1">
         <v>44926</v>
       </c>
@@ -4008,61 +4008,61 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A367" s="1"/>
     </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A368" s="1"/>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A369" s="1"/>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A370" s="1"/>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A371" s="1"/>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A372" s="1"/>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A373" s="1"/>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A374" s="1"/>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A375" s="1"/>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A376" s="1"/>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A377" s="1"/>
     </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A378" s="1"/>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A379" s="1"/>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A380" s="1"/>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A381" s="1"/>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A382" s="1"/>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A383" s="1"/>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A384" s="1"/>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385" s="1"/>
     </row>
   </sheetData>
@@ -4072,18 +4072,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4290,18 +4290,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC537D72-CE20-4DBB-BAE3-4B3C88518F3C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668E6B46-E1D2-4884-8947-5A667A68A9D5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668E6B46-E1D2-4884-8947-5A667A68A9D5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC537D72-CE20-4DBB-BAE3-4B3C88518F3C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>